<commit_message>
[sofi_functions.guess_missing_BWs] copied the function from actor_utils for testing
</commit_message>
<xml_diff>
--- a/tests/GPCRmd_B2AR_nomenclature_test.xlsx
+++ b/tests/GPCRmd_B2AR_nomenclature_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofitiwari/work_Charite/sofi_functions/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4E875D-0D5F-774A-B73B-B262307BC335}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08B7683-A9EE-9642-85C1-60739F1030B4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>1x26</t>
   </si>
   <si>
-    <t>E27</t>
-  </si>
-  <si>
     <t>1x27</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>S262</t>
+  </si>
+  <si>
+    <t>E27</t>
   </si>
 </sst>
 </file>
@@ -502,9 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C256"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
@@ -535,29 +533,29 @@
         <v>1.26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>1.27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>1.28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
Updated the test file GPCRmd_B2AR_nomenclature.xlsx to add more rows
</commit_message>
<xml_diff>
--- a/tests/GPCRmd_B2AR_nomenclature_test.xlsx
+++ b/tests/GPCRmd_B2AR_nomenclature_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofitiwari/work_Charite/sofi_functions/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08B7683-A9EE-9642-85C1-60739F1030B4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E913D8A-3C6F-154D-90D0-C35426776D7F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>TM1</t>
   </si>
@@ -52,6 +52,60 @@
   </si>
   <si>
     <t>E27</t>
+  </si>
+  <si>
+    <t>M40</t>
+  </si>
+  <si>
+    <t>S41</t>
+  </si>
+  <si>
+    <t>L42</t>
+  </si>
+  <si>
+    <t>I43</t>
+  </si>
+  <si>
+    <t>V44</t>
+  </si>
+  <si>
+    <t>L45</t>
+  </si>
+  <si>
+    <t>A46</t>
+  </si>
+  <si>
+    <t>I47</t>
+  </si>
+  <si>
+    <t>V48</t>
+  </si>
+  <si>
+    <t>1x29</t>
+  </si>
+  <si>
+    <t>1x30</t>
+  </si>
+  <si>
+    <t>1x31</t>
+  </si>
+  <si>
+    <t>1x33</t>
+  </si>
+  <si>
+    <t>1x34</t>
+  </si>
+  <si>
+    <t>1x35</t>
+  </si>
+  <si>
+    <t>1x32</t>
+  </si>
+  <si>
+    <t>1x36</t>
+  </si>
+  <si>
+    <t>1x37</t>
   </si>
 </sst>
 </file>
@@ -500,9 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C256"/>
+  <dimension ref="A1:C255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
@@ -558,50 +614,104 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+    <row r="6" spans="1:3" ht="14">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.43</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.44</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.47</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2"/>
@@ -714,12 +824,12 @@
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="A37" s="1"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="1"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2"/>
@@ -872,12 +982,12 @@
       <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="A69" s="1"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="1"/>
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="2"/>
@@ -1055,12 +1165,12 @@
       <c r="C105" s="2"/>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
+      <c r="A106" s="1"/>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="1"/>
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="2"/>
@@ -1193,12 +1303,12 @@
       <c r="C133" s="2"/>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
+      <c r="A134" s="1"/>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="1"/>
+      <c r="A135" s="2"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="2"/>
@@ -1406,12 +1516,12 @@
       <c r="C176" s="2"/>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="2"/>
-      <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
+      <c r="A177" s="1"/>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" s="1"/>
+      <c r="A178" s="2"/>
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="2"/>
@@ -1599,12 +1709,12 @@
       <c r="C215" s="2"/>
     </row>
     <row r="216" spans="1:3">
-      <c r="A216" s="2"/>
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
+      <c r="A216" s="1"/>
     </row>
     <row r="217" spans="1:3">
-      <c r="A217" s="1"/>
+      <c r="A217" s="2"/>
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="2"/>
@@ -1727,12 +1837,12 @@
       <c r="C241" s="2"/>
     </row>
     <row r="242" spans="1:3">
-      <c r="A242" s="2"/>
-      <c r="B242" s="2"/>
-      <c r="C242" s="2"/>
+      <c r="A242" s="1"/>
     </row>
     <row r="243" spans="1:3">
-      <c r="A243" s="1"/>
+      <c r="A243" s="2"/>
+      <c r="B243" s="2"/>
+      <c r="C243" s="2"/>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="2"/>
@@ -1793,11 +1903,6 @@
       <c r="A255" s="2"/>
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
-    </row>
-    <row r="256" spans="1:3">
-      <c r="A256" s="2"/>
-      <c r="B256" s="2"/>
-      <c r="C256" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
[sofi_tests_by_unittest.Test_guess_missing_BWs] test added but need to attain 100% coverage
</commit_message>
<xml_diff>
--- a/tests/GPCRmd_B2AR_nomenclature_test.xlsx
+++ b/tests/GPCRmd_B2AR_nomenclature_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofitiwari/work_Charite/sofi_functions/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E913D8A-3C6F-154D-90D0-C35426776D7F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA65BCA4-0A29-EF40-BFC4-3C6394C310F7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:C255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>

</xml_diff>